<commit_message>
City index 25-9 complete.
</commit_message>
<xml_diff>
--- a/data_indexpoints_tidy/tallmateriale_19955.xlsx
+++ b/data_indexpoints_tidy/tallmateriale_19955.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Programmering\R\byindeks\data_indexpoints_tidy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA67D16-26F4-4E98-911A-8BC4A693ECAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED1C17C-C90E-41AB-9A2D-B530465B0186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21150" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="77040" windowHeight="21390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="punkt_adt" sheetId="1" r:id="rId1"/>
@@ -651,9 +651,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -706,7 +706,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -759,7 +759,7 @@
         <v>1750</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -812,7 +812,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -865,7 +865,7 @@
         <v>3060</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -918,7 +918,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -971,7 +971,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>1960</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -1245,11 +1245,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6:L6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="5.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1287,7 +1298,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -1316,7 +1327,7 @@
         <v>5.79</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1354,7 +1365,7 @@
         <v>5.47</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1392,7 +1403,7 @@
         <v>1.85</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -1415,7 +1426,7 @@
         <v>1.08</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1441,7 +1452,7 @@
         <v>20.38</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -1479,7 +1490,7 @@
         <v>4.4800000000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -1514,7 +1525,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1534,7 +1545,7 @@
         <v>10.08</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>61</v>
       </c>
@@ -1581,11 +1592,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>75</v>
       </c>
@@ -1629,7 +1640,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2024</v>
       </c>

</xml_diff>